<commit_message>
updated handling of uploads by implementing a dual-client approach in supabase
</commit_message>
<xml_diff>
--- a/uploads/template_student_data.xlsx
+++ b/uploads/template_student_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wccvicedu-my.sharepoint.com/personal/leed_e_wcc_vic_edu_au/Documents/Homeroom/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E28083-2A78-4AAD-8B5D-0E93A43D2950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{E8E28083-2A78-4AAD-8B5D-0E93A43D2950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE1A5783-5883-4051-8A26-BD6DC50340CF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA61B80E-0392-4D06-90DD-9D43CDF00CCC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CA61B80E-0392-4D06-90DD-9D43CDF00CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="172">
   <si>
     <t>student_name</t>
   </si>
@@ -60,19 +60,725 @@
   </si>
   <si>
     <t>adjectives</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Sereana</t>
+  </si>
+  <si>
+    <t>Josiah</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Cassius</t>
+  </si>
+  <si>
+    <t>Keziah</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Michaela</t>
+  </si>
+  <si>
+    <t>Caleb</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Aidan</t>
+  </si>
+  <si>
+    <t>Sherin</t>
+  </si>
+  <si>
+    <t>Serah</t>
+  </si>
+  <si>
+    <t>Capri</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Caitlyn</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Annabelle</t>
+  </si>
+  <si>
+    <t>Ian</t>
+  </si>
+  <si>
+    <t>Adora</t>
+  </si>
+  <si>
+    <t>Jarell</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>Domenic</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>10B</t>
+  </si>
+  <si>
+    <t>Encourage to get involved in extracurriculars, has potential if he chooses to step up more - as evident in the amount he assisted the Fundraiser, encourage to invest in faith.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jayden is a lively student who enjoys spending time with his friends and is a valued member of our home group. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Jayden has been an active participant in the volleyball program this semester, showcasing his teamwork and athletic skills. He has shown significant improvement and effort in Art, a subject he initially felt less confident about. This determination is commendable and reflects his willingness to step out of his comfort zone. In subjects like Maths and Engineering, Jayden has made decent efforts, demonstrating a solid understanding of the material. However, he has been less consistent with his test preparation in some subjects, which has impacted his performance. It is crucial for Jayden to set aside regular study time to prepare for tests and assessments to ensure steady progress across all areas. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>I also encourage Jayden to see his value in Christ, and invest time building his faith through reading more of the Scripture and engaging in conversations about God outside of a Church environment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Keep up the hard work, Jayden, and continue to develop your study habits and take advantage of the opportunities available in the second half of the year.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cheerful, Sociable</t>
+  </si>
+  <si>
+    <t>Was a good participant for Finney in House Athletics.</t>
+  </si>
+  <si>
+    <t>Enjoyed Environmental Science, Enjoyed Marine Biology, Been doing fairly well across board with some room for improvement if improve study techniques.</t>
+  </si>
+  <si>
+    <t>Sociable</t>
+  </si>
+  <si>
+    <t>Outgoing, Sociable</t>
+  </si>
+  <si>
+    <t>Made the most of work experience by going to Air Force in Northern Territory</t>
+  </si>
+  <si>
+    <t>Done well to invest in School Basketball team and be an active participant in sports events.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Joshua has shown commendable dedication and enthusiasm throughout Semester One. His active involvement in interschool Cross Country highlights his passion for Physical Education and his commitment to staying physically active. Academically, Joshua has demonstrated a keen interest in Engineering and has made notable improvements in Maths. As Joshua continues to develop these study habits, they will be instrumental in his ongoing success. I encourage Joshua to maintain this positive momentum and continue engaging with his peers and teachers. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Lastly, I encourage Joshua to find opportunities to strengthen himself personally by continuing to build his relationship with Christ, doing so by reading more of the Scripture and engaging in discussions about God outside of a Church environment. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Keep up the excellent work, Joshua, and best wishes for the second half of the year!</t>
+    </r>
+  </si>
+  <si>
+    <t>Made good efforts across board, particularly enjoyed learning about chemistry in science and making improvements in Psychology.</t>
+  </si>
+  <si>
+    <t>Enthusiastic, Well-mannered</t>
+  </si>
+  <si>
+    <t>Enjoyed Science. Did fairly well in chemistry. Could make some improvements across subjects by refining study techniques.</t>
+  </si>
+  <si>
+    <t>Welcome addition to School since new student, Encourage investment in faith</t>
+  </si>
+  <si>
+    <r>
+      <t>Isaac</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is a lively student who enjoys spending time with his friends and is a valued member of our home group. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">He has demonstrated a strong interest in Physical Education, actively participating in sports teams such as Volleyball and Netball. His confidence shines through in these activities, inspiring his teammates and contributing to a dynamic team spirit. In the classroom, Isaac brings the same enthusiasm and energy, showing good effort across many of his subjects. To further enhance his academic performance, it is important for Isaac to set aside dedicated time to study and prepare for tests and assessments. This disciplined approach will enable him to achieve his full potential. Isaac is encouraged to continue building on these skills, as they will be crucial for his success in the future. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>I also encourage Isaac to seek and understand how his worth is not defined by his academics, nor by his friends, but in him being a child of God, truly and dearly loved.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Keep up the excellent work, Isaac, and continue to strive for balance and excellence in all areas during the second half of the year.</t>
+    </r>
+  </si>
+  <si>
+    <t>Amicable, Thoughtful</t>
+  </si>
+  <si>
+    <t>Enjoyed making progress in Mathematics, and visiting the Holocaust Museum for History. Done quite well across his subjects</t>
+  </si>
+  <si>
+    <t>Plays in Basketball team. Could invest elsewhere, he has a lot to offer and lots of skills to build.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Isaac has demonstrated exceptional dedication and enthusiasm both inside and outside the classroom throughout this semester. His active involvement in Musiquest showcases his passion for music and willingness to explore his creative talents. Furthermore, Isaac's high participation in House Swimming and House Athletics exemplifies his commitment to sporting activities and team spirit. In addition to his extracurricular engagements, Isaac has shown a genuine enjoyment for Physical Education, actively participating and contributing positively to class activities. His interest in astronomy within the Science curriculum highlights his curiosity about the world around him and his eagerness to delve into new topics. Isaac's academic efforts have remained consistently strong across all subjects, reflecting his diligent work ethic and dedication to learning. With his enthusiasm for learning and active involvement in various activities, Isaac is well-positioned for continued success in the upcoming semester. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>I also encourage Isaac to see his value in Christ, and invest time building his faith through reading more of the Scripture and engaging in conversations about God outside of a Church environment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Keep up the outstanding work, Isaac!</t>
+    </r>
+  </si>
+  <si>
+    <t>No interest in investing in any opportunities offered. Would strongly encourage him to push himself outside his comfort zone as this can help him learn new skills and perspectives that will be invaluable to life.</t>
+  </si>
+  <si>
+    <t>Inconsisent scores. Seems to lack any particular drive in any subject.</t>
+  </si>
+  <si>
+    <t>Encourage to seek a mentor. Learn what value he has in God's eyes, and build a deeper understanding of what the Gospel means.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caleb is a well-mannered and sociable student who enjoys the company of friends. This semester he has taken a particular interest in English, and has enjoyed learning about film analysis. His academic efforts in most other subjects do require more attention though. Caleb can benefit by communicating more with his teachers, and voicing immediately when he doesn’t fully understand something. This was something that has been more difficult to do lately due to the online learning environment. I encourage Caleb to not get disheartened by his marks, but also not to completely give up on school either. He has a lot of potential, and teachers have noticed improvement in marks when he seeks to deeply understand a topic. I also encourage Caleb to continue seeking what else he can be good at, and develop a wide range of skills that can fully prepare him for life. As he enters the second half of High School, Caleb should make the most of his time by continuing to enjoy his friendships, and by building a deeper relationship with God. All the best Caleb!  </t>
+  </si>
+  <si>
+    <t>Well mannered, kind hearted</t>
+  </si>
+  <si>
+    <t>Enjoys science, could improve academics by opening more dialogue with her teachers and asking questions</t>
+  </si>
+  <si>
+    <t>None. Could consider what things she might want to invest in.</t>
+  </si>
+  <si>
+    <t>Michaela commented on how she has improved her ability to talk to more people that i usually wouldnt talk to. Keep this up</t>
+  </si>
+  <si>
+    <t>Esther is a kind, considerate student and our Home Group has been blessed to have her presence with us this semester. Out of all her classes, she has particularly enjoyed the relaxed nature and the activities done in Drama. In the past, Esther’s efforts in her subjects have been inconsistent. She has noted that English has been one of these subjects she has struggled in. However, Esther noted that this semester she really engaged with the content matter in English, and really enjoyed learning about the history related to Morris Gleitzmann’s “Once”. I encourage Esther to continue engaging in her subjects in this way, by finding and relating the concepts to things she is interested in. In Home Group, Esther presented a wonderful devotional about worship, and how it is important not to be ashamed to worship God when around others. I encourage Esther to continue to learn more inspiring lessons from the Bible as she continues on her faith journey. In the years ahead, I also encourage Esther to build a strong confidence in herself. When confident, Esther holds the potential to positively influence those around her. For this reason, I encourage Esther to apply herself in the years ahead, and seek opportunities where she can demonstrate leadership. All the best for the years ahead, Esther!</t>
+  </si>
+  <si>
+    <t>Lively</t>
+  </si>
+  <si>
+    <t>Done well to connect with others over the course of just one term. Displays a strong dedication to God.</t>
+  </si>
+  <si>
+    <t>Not involved in any yet, would encourage to seek some out, such as the Student-run Prayer Groups or Make Poverty History.</t>
+  </si>
+  <si>
+    <t>Well-mannered, Kind-Hearted</t>
+  </si>
+  <si>
+    <t>Science Talent Search, Debating, Was great up-front in Musiquest, Wood Club</t>
+  </si>
+  <si>
+    <t>Enjoyed History. Doing well across the board</t>
+  </si>
+  <si>
+    <t>Consider ways to grow leadership skills</t>
+  </si>
+  <si>
+    <t>Toby is a kind-hearted and amicable student who consistently exhibits a positive demeanour in the classroom. His friendly nature makes it effortless for his peers to connect with him, and it is evident that he highly values his friendships. Toby maintains a dedicated and diligent approach to his studies across all subjects, consistently communicating with his teachers to ensure his progress. This semester, he has displayed a keen interest in Engineering, expressing his enjoyment in creating his own autonomous vehicles. Toby has excelled in multiple other subjects, actively participating with great enthusiasm. Additionally, it has been great to see Toby extend himself by getting involved in so many extra-curricular activities, including House and inter-school debating, chess, and Science Talent Search to name a few. While Toby progresses through secondary college, I encourage him to continue nurturing his personal growth through his faith journey, and do such through reading the scripture. I can imagine that Toby would engage well with theological discussions, and would encourage him to have them. Beyond this, I have no doubt that Toby's positive attitude and cooperative nature will continue to contribute to a harmonious learning environment. Best wishes for the upcoming semester, Toby</t>
+  </si>
+  <si>
+    <t>Logan is a polite student who always shows a positive attitude in class. He holds a friendly nature that makes it easy for other students to get along with him, and it is clear that he highly values his friends. This semester he has noted to particularly enjoy Media, stating that he enjoys creating pictures. Logan could however benefit in his academics by learning not to rush his work, and slowly digest the content given to him by taking brief notes. I also encourage Logan to put in place some good study techniques that can help him with exams and tests. During Homegroup this semester, Logan presented a deep theological discussion about the purpose of the flood in Genesis. I encourage Logan to continue to take scripture and faith as seriously as what he has been displaying thus far, and to initiate and engage in theological discussions outside of the common Church environment. Furthermore, I also encourage Logan to continue to be positive influence on his peers, and to see the leadership potential he can bring to his community. All the best for the next semester, Logan!</t>
+  </si>
+  <si>
+    <t>Sociable, Cheerful</t>
+  </si>
+  <si>
+    <t>School Production. Hope gets a lot out of that.</t>
+  </si>
+  <si>
+    <t>Enjoyed Psychology. Doing pretty well in some subjects like Maths and Psychology, though could work to improve communication with some teachers for other subjects.</t>
+  </si>
+  <si>
+    <t>Invest in Faith</t>
+  </si>
+  <si>
+    <t>Good to see involvement in Chapel Band</t>
+  </si>
+  <si>
+    <t>Could invest in some. Shows great potential in developing leadership, as evident in how he committed himself thoroughly in the Fundraiser</t>
+  </si>
+  <si>
+    <t>Keep investing in faith, good to hear that he's doing daily bible reading.</t>
+  </si>
+  <si>
+    <t>Doing fairly well across subjects, enjoyed science</t>
+  </si>
+  <si>
+    <t>Max is a commendable student who consistently demonstrates a positive attitude in the classroom. It was great to see his enthusiasm and determination at the swimming carnival as he participated in swimming events. In terms of academics, Max has shown a strong interest in Science and Geography. This interest has translated into commendable academic performance in these subjects. However, recently, Max has become a quieter presence in the classroom. It would be beneficial to hear more from him during class discussions to leverage his insights and perspectives. Encouraging Max to share his thoughts will not only contribute to his own growth but also enhance the learning experience for his peers. By actively participating, Max can enrich the collaborative and interactive nature of the classroom. Overall, Max has exhibited admirable qualities as a student. It has been great to see his involvement in extracurricular activities such as Badminton club has been. As he continues on in Secondary College I encourage Max to find opportunities to strengthen himself personally by continuing to build his relationship with Christ, doing so by reading more of the Scripture and engaging in discussions about God outside of a Church environment. All the best for the next semester, Max!</t>
+  </si>
+  <si>
+    <t>Sociable, Lively</t>
+  </si>
+  <si>
+    <t>Outgoing, thoughtful</t>
+  </si>
+  <si>
+    <t>Enjoyed Financial Stewardship and Psychology. Doing fairly well across board, but might benefit in refining study techniques.</t>
+  </si>
+  <si>
+    <t>Keep building leadership skills, and keep investing in faith. Was very helpful during the Fundraiser and showed great servanet leadership.</t>
+  </si>
+  <si>
+    <t>John is a very conscientious and thoughtful student who always applies himself academically as well as in all other areas of his life. He has shown a devoted love for learning new things, and enjoys solving problems. He has especially enjoyed Science this semester, as well as the chance to lead younger students in Sport Science. I encourage John to keep giving things a go, and perhaps strive for the Duke of Edinburgh’s award next year. John has also been very good at communicating with his teachers and asking questions in class. Going forward I encourage John to continue seeking out how he can develop skills in leadership, and become a stronger influence amongst his community. Provided he builds more confidence, he has enormous potential to positively affect those around him, both people close to him and those not. All the best for the years ahead, John!</t>
+  </si>
+  <si>
+    <t>Involved in badminton club. Would suggest Make Poverty History Club for him.</t>
+  </si>
+  <si>
+    <t>Bright student, has potential to achieve really well, but needs to get used to putting in more effort than what he might have needed in past.</t>
+  </si>
+  <si>
+    <t>Sociable, Intelligent</t>
+  </si>
+  <si>
+    <t>Independent</t>
+  </si>
+  <si>
+    <t>Enjoyed Sport Science and Media, as well as Personal Development. Would encourage more open dialogue with teachers to help understand how to best approach each subject.</t>
+  </si>
+  <si>
+    <t>Good to see involvement in string ensemble.</t>
+  </si>
+  <si>
+    <t>Keep putting yourself out there Socially</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caleb is a well-mannered student . This semester he has taken a particular interest in English, and has enjoyed learning about film analysis. His academic efforts in most other subjects do require more attention though. Caleb can benefit by communicating more with his teachers, and voicing immediately when he doesn’t fully understand something. This was something that has been more difficult to do lately due to the online learning environment. I encourage Caleb to not get disheartened by his marks, but also not to completely give up on school either. He has a lot of potential, and teachers have noticed improvement in marks when he seeks to deeply understand a topic. I also encourage Caleb to continue seeking what else he can be good at, and develop a wide range of skills that can fully prepare him for life. As he enters the second half of High School, Caleb should make the most of his time by continuing to enjoy his friendships, and by building a deeper relationship with God. All the best Caleb!  </t>
+  </si>
+  <si>
+    <t>Art Design Club, Cross Country, Hope gets a lot out of these</t>
+  </si>
+  <si>
+    <t>Enjoyed the topics taught in science and HHD, Enjoyed the challenge found in Maths. Done well in her subjects.</t>
+  </si>
+  <si>
+    <t>Kind-Hearted, Polite</t>
+  </si>
+  <si>
+    <t>Good work on keeping up with bible readings</t>
+  </si>
+  <si>
+    <t>Lydia is a considerate and assiduous student who does well to always look outwardly and consider those around her. She does very well academically, and has particularly enjoyed the relaxed nature found in Drama. She also very much enjoyed the excursion to see “Hairspray” live with her Drama class. Lydia also does extremely well to get herself involved in school culture outside of the classroom, participating in many musical groups such as Senior Choir and Concert Band. Lydia also did extremely well to earn a Bursary for her Science Talent Search report. Lydia also does well to be a positive influence on her peers. She demonstrates a strong faith in God, as evident in her actions and in the devotion she gave in Home Group about Forgiveness. It is encouraging to hear her describe her relationship with God so personally. I encourage Lydia as she progresses throughout high school to be evangelical with this love she has for the Lord, and to openly express it in the hopes that her peers around her can also come to know Christ. All the best for the years ahead Lydia!</t>
+  </si>
+  <si>
+    <t>Polite, Dedicated</t>
+  </si>
+  <si>
+    <t>Art Design Club</t>
+  </si>
+  <si>
+    <t>Enjoyed Marine Biology and Science, especially the Wildlife Expo Incursion</t>
+  </si>
+  <si>
+    <t>Hannah is a considerate and assiduous student who does well to always look outwardly and consider those around her. She does very well academically, and has particularly enjoyed studying chemistry in science this semester. Hannah also does extremely well to get herself involved in school culture outside of the classroom, participating in groups like Make Poverty History and the Engineering Club. She also did extremely well to earn a Bursary for her Science Talent Search report. Hannah also does well to be a positive influence on her peers. She does not noticeably show concern for how others think of her, and holds an encouraging and outgoing attitude making her very friendly and approachable. In Home Group, Hannah presented a great devotion about Forgiveness. I encourage Hannah to continue to learn more inspiring lessons from the Bible as she continues on her faith journey. Going forward, I encourage Hannah to seek and understand how her worth is not defined by her academics, nor by her friends, but in her being a child of God. All the best for the next year, Hannah!</t>
+  </si>
+  <si>
+    <t>Keep up the habit of reading the bible. Keep applying yourself and finding ways to develop a broad range of skills.</t>
+  </si>
+  <si>
+    <t>Kind, Lively, Outgoing</t>
+  </si>
+  <si>
+    <t>Has done particularly well in Architechure and History</t>
+  </si>
+  <si>
+    <t>Makes great use of opportunities at school, including musiquest, chapel team, choir, school production, string ensemble.</t>
+  </si>
+  <si>
+    <t>Seek out and learn leadership skills - Has a lot to offer. Keep investing in faith as she currently is, and invest in the faith of her peers.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ciara is a considerate and assiduous student who does well to always look outwardly and consider those around her. Ciara’s efforts across his subjects have been quite positive, but she has most enjoyed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>English, Physical Education, and Health.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> She has also enjoyed learning about God’s Design in Science. I encourage Ciara to consider taking up the Duke of Edinburgh’s award next year, as it will probably lead to some beneficial personal development. Ciara does very well to be a positive influence on her peers. She demonstrates a strong faith in God as evident in her actions. It is encouraging to hear her describe her relationship with God so personally. I encourage Ciara that as she progresses throughout high school to be evangelical with this love she has for the Lord, and to openly express it in the hopes that her peers around her can also come to know Christ. I also encourage Ciara to seek out how she can develop skills in leadership, and become a stronger influence amongst his community. More than what she might realise, she has enormous potential to positively affect those around her, both people close to her and those not. All the best for the years ahead Ciara!</t>
+    </r>
+  </si>
+  <si>
+    <t>Polite, kind-hearted</t>
+  </si>
+  <si>
+    <t>Enjoyed fine art and PE</t>
+  </si>
+  <si>
+    <t>None, though might want to consider Art Club.</t>
+  </si>
+  <si>
+    <t>Angela is a very polite and considerate student who often thinks of others. She is to be commended for the development she has shown this past semester in giving tasks a good go. Angela particularly enjoyed the chances to cook in food studies this past semester, as well as the opportunity to learn about diseases in Science. . I encourage Angela to adopt goal setting strategies where needed if completing tasks can ever pose to be a challenge. I encourage Chantel to continue to draw closer to God and grow in His wisdom.</t>
+  </si>
+  <si>
+    <t>Invest in faith</t>
+  </si>
+  <si>
+    <t>Done well thus far, Most enjoyed Psychology</t>
+  </si>
+  <si>
+    <t>Art Club, Badminton Club, Active participant for house in Athletics and Swimming</t>
+  </si>
+  <si>
+    <t>Well-mannered, harmonious</t>
+  </si>
+  <si>
+    <t>Enjoyed Food Studdies, Struggled in science and History.</t>
+  </si>
+  <si>
+    <t>Keep investing in faith. Make sure to always open dialogue with teachers when needed.</t>
+  </si>
+  <si>
+    <t>Enjoyed science and history, done well in most</t>
+  </si>
+  <si>
+    <t>Considerate, Harmonious</t>
+  </si>
+  <si>
+    <t>Anngraha is a very courteous and polite student who holds a good attitude to her school and to her peers around her. She has been doing well across multiple subjects, and has particularly enjoyed Mathematics, Science, and the chance to learn about diseases. It hasbeen great to see Anngraha maintain a good work ethic and ask questions when needed. It’s also been great to see her faith displayed through her kindness, as well as through the devotion she presented to the Home Group about faith concurring fear. I encourage Anngraha to continue to apply herself not just in her school work, but in overall classroom discussions, in her social life, and in all other aspects of her life!</t>
+  </si>
+  <si>
+    <t>Keep investing in faith, good to hear the interest put towards it.</t>
+  </si>
+  <si>
+    <t>School Production, Library Volunteer, chapel team</t>
+  </si>
+  <si>
+    <t>Making good use of opportunities at school, with art club, school production, senior choir, musiquest. Very creative</t>
+  </si>
+  <si>
+    <t>Lively, polite</t>
+  </si>
+  <si>
+    <t>Done well in all. Enjoyed history and architecture.</t>
+  </si>
+  <si>
+    <t>It sound like she's working on trying to make her faith her own, which is excellent</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ciara is a considerate and assiduous student who does well to always look outwardly and consider those around her. Ciara’s has most enjoyed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>English, Physical Education, and Health.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> She has also enjoyed learning about God’s Design in Science. I encourage Ciara to consider taking up the Duke of Edinburgh’s award next year, as it will probably lead to some beneficial personal development. Ciara does very well to be a positive influence on her peers. She demonstrates a strong faith in God as evident in her actions. It is encouraging to hear her describe her relationship with God so personally. I encourage Ciara that as she progresses throughout high school to be evangelical with this love she has for the Lord, and to openly express it in the hopes that her peers around her can also come to know Christ. I also encourage Ciara to seek out how she can develop skills in leadership, and become a stronger influence amongst his community. More than what she might realise, she has enormous potential to positively affect those around her, both people close to her and those not. All the best for the years ahead Ciara!</t>
+    </r>
+  </si>
+  <si>
+    <t>Well-mannered, independent</t>
+  </si>
+  <si>
+    <t>Enjoyed science, did well in some such as psychology, struggled in mathematics</t>
+  </si>
+  <si>
+    <t>Good participant at athletics and sport events</t>
+  </si>
+  <si>
+    <t>Keep learning new skills</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kayla is a hard-working student who does well to make the most of her time at Waverley Christian College. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Kayla has been actively engaged in various sporting activities this semester, including representing the school in interschool cross country, the soccer team, and participating in numerous events during House Athletics. In addition to her extracurricular pursuits, Kayla has shown a genuine enjoyment of Physical Education and Mathematics, consistently displaying enthusiasm and a positive attitude towards learning in these subjects. Kayla has maintained commendable academic performance across all subjects, reflecting her diligence and hard work. I encourage Kayla to continue developing the study habits she has been cultivating, as they will serve as valuable assets in managing her academic workload effectively. By prioritizing consistent study routines, Kayla can further enhance her academic achievements while continuing to excel in her extracurricular pursuits. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>I also encourage Kayla to seek and understand how her worth is not defined by her academics, nor by her friends, but in her being a child of God, truly and dearly loved.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Keep up the excellent work, Kayla!</t>
+    </r>
+  </si>
+  <si>
+    <t>Encourage to get more involved in extracurriculars for purpose of developing new skills and perspectives</t>
+  </si>
+  <si>
+    <t>Sociable, independent</t>
+  </si>
+  <si>
+    <t>Enjoyed Mathematics, struggled with chemistry in science, encourage to put more structure to how she studdies to get the most out of VCE</t>
+  </si>
+  <si>
+    <t>Good to hear she volunteers for Kids Church</t>
+  </si>
+  <si>
+    <t>Faith is a friendly student who enjoys all aspects of social life. It has been great having Faith in our Home Group this year. Her efforts in her academics have been somewhat inconsistent, and thus I encourage Faith to learn to use effective study techniques to help him in the future, such as the prioritization of practice questions when revising. Faith has a lot of potential to apply herself outside of the classroom. I highly encourage Faith to find out what sort of extracurricular activity she might enjoy and be open minded as to the enjoyment she can get out of new activities. As she continues on in Secondary School, I encourage Faith to find opportunities to strengthen herself personally by continuing to build her relationship with Christ, and by reading more of the Scripture. Faith can also build this relationship by engaging in conversations about Christ with her peers outside of the Church setting. All the best for the next semester, Faith!</t>
+  </si>
+  <si>
+    <t>Addyson is a very sociable student who enjoys the company of friends. She has done very well to achieve consistently good results across all her subjects, though this semester she has particularly enjoyed Food Studies. Addyson has noted that she employed a lot of effective study skills to make great improvement in subjects such as Mathematics. What is positive to see is the way Addyson interacts with her friends, as she has surrounded herself with a very supportive friendship group. I encourage Addyson to also interact with people she does not know as well and broaden her social connections. Addyson also presented a good devotion in Home Group about Patience. I encourage Addyson to continue to find opportunities to strengthen her relationship with God. All the best for the years ahead Addyson!</t>
+  </si>
+  <si>
+    <t>Cheerful, Dilligent</t>
+  </si>
+  <si>
+    <t>Enjoyed Legal Studdies. Done well in all subjects. Is proactive in communication with teachers.</t>
+  </si>
+  <si>
+    <t>Great to see involvement in the debating team, he's a good fit</t>
+  </si>
+  <si>
+    <t>Kevin does well to look out for others, I encourage him to keep doing this more and keep developing his leadership skills</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Max is a kind-hearted and amicable student who consistently exhibits a positive demeanour in the classroom. His friendly nature makes it effortless for his peers to connect with him, and it is evident that he highly values his friendships. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Max has displayed a genuine passion for Physical Education, Art, and Science, actively participating and demonstrating enthusiasm for these subjects throughout the semester. His dedication to his academics is commendable, as he consistently applies himself across all subjects with diligence and effort. While excelling in his studies, I encourage Max to consider further enriching his school experience by engaging in extracurricular activities. Participation in clubs or events beyond the classroom can provide valuable opportunities for personal growth, leadership development, and the exploration of new interests. I also encourage Max to engage in discussions about Christ with his peers outside of the regular Church setting. Such discussions will both help build Max’s knowledge of the Bible, as well as allow him to be an influence on others. Keep up the excellent work, Max, and continue to explore and embrace new avenues for growth and involvement!</t>
+    </r>
+  </si>
+  <si>
+    <t>Enjoyed Extended Investigations and English. Struggled in Science and Mathematics.</t>
+  </si>
+  <si>
+    <t>Polite, Considerate</t>
+  </si>
+  <si>
+    <t>Good to see involvement in Basketball team</t>
+  </si>
+  <si>
+    <t>New to school, but has done well to establish himself.</t>
+  </si>
+  <si>
+    <t>Reubin is to be commended for his competent, mature approach to school life this term. He is a courteous student who has already shown to make a good effort in catching up on much of the work he missed during his transition to a new school. He has noted to have particularly enjoyed studying Science and Maths. I encourage Reubin to keep the persistent and positive attitude he has been demonstrating as he continues adjusting to this new school. I also encourage Reubin to consider taking up the Duke of Edinburgh’s award next year, as it will probably lead to some beneficial personal development. Waverley is very fortunate to have him as a student. It was also great to hear Reubin share about his faith, and I encourage him to keep building it through reading more of the Scripture and engaging in conversations about God outside of a Church environment. Best wishes for next semester, Paul!</t>
+  </si>
+  <si>
+    <t>Enjoyed Legal Studdies, Enjoyed Food Studdies, Struggled in science</t>
+  </si>
+  <si>
+    <t>Encourage to keep getting involved in extra curriculas. Good to see involvement in Musiquest</t>
+  </si>
+  <si>
+    <t>Independent, well mannered</t>
+  </si>
+  <si>
+    <t>Keep investing in faith, have faith-based discussions outside of regular church setting.</t>
+  </si>
+  <si>
+    <t>Kaedan is a bright and considerate student who contributes to Home Group in a lively and positive manner. Kaedan has done very well to consistently get high academic results, but has most enjoyed Science and learning various topics such as Chemistry. He is also to be commended for achieving a distinction for his report in the Science Talent Search. Kaedan has surrounded himself with a good network of friends who hold a positive influence on him. Kaedan himself carries a friendly nature that makes it easy for other students to get along with him. As he continues in Secondary, I encourage Kaedan to keep pushing himself beyond his comfort zones, both socially and academically, as he has the potential to become an even more well-rounded individual as he continues to try new things and expand his abilities. In Home Group, Kaedan presented a great devotion about Procrastination. I encourage Kaedan to continue to learn more inspiring lessons from the Bible as he continues on his faith journey. I also encourage Kaedan to seek and understand how his worth is not defined by his academics, nor by his friends, but in him being a child of God, truly and dearly loved. All the best for the years ahead, Kaedan!</t>
+  </si>
+  <si>
+    <t>Amicable, Dilligent</t>
+  </si>
+  <si>
+    <t>Does well to get himself involved in Debating Team, Science Talent Search and Chapel Band</t>
+  </si>
+  <si>
+    <t>Enjoyed Math Methods and Legal Studdies, done well in all</t>
+  </si>
+  <si>
+    <t>Thoughtful, Polite</t>
+  </si>
+  <si>
+    <t>Make sure to keep openining dialogue with teachers when needed. Invest in faith and have discussions with that with mentores.</t>
+  </si>
+  <si>
+    <t>Enjoyed English and Bible</t>
+  </si>
+  <si>
+    <t>Senior Choir, Badminton Club</t>
+  </si>
+  <si>
+    <t>Enjoyed Applied Computing, did well in most.</t>
+  </si>
+  <si>
+    <t>Encourage to find ways to put herself out there, she has a lot to offer</t>
+  </si>
+  <si>
+    <t>Enjoyed Physical Education, done well in most</t>
+  </si>
+  <si>
+    <t>Make sure to keep communicating with teachers.</t>
+  </si>
+  <si>
+    <t>Made good investment in sports teams</t>
+  </si>
+  <si>
+    <t>Lively, independent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,8 +801,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,24 +1151,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B70A5B5-45BB-4225-8A4B-0CDB29467C86}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="186.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="118.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="186.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="118.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,6 +1192,760 @@
       </c>
       <c r="H1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" t="s">
+        <v>163</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>